<commit_message>
2.3.1: Release DyanamicClause definition feature now!
</commit_message>
<xml_diff>
--- a/meta/program/blancoDbTask.xlsx
+++ b/meta/program/blancoDbTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED783D5-9668-0848-B6C1-751E2AC74D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAD6C5D-C0DE-0F44-B12E-9C461BA3AC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17040" yWindow="740" windowWidth="19760" windowHeight="18360" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -347,29 +347,6 @@
   </si>
   <si>
     <t>行末記号をしていします。LF=0x0a, CR=0x0d, CFLF=0x0d0x0a とします。LFがデフォルトです。</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>verbose</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>自動生成に関する詳細な情報を出力します。</t>
-    <rPh sb="0" eb="1">
-      <t xml:space="preserve">ジドウセイセイジノ </t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t xml:space="preserve">カンスル </t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t xml:space="preserve">ショウサイナ </t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t xml:space="preserve">ジョウホウヲ </t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t xml:space="preserve">シュツリョクシマス。 </t>
-    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -820,36 +797,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -868,6 +815,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,8 +1216,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1284,10 +1261,10 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1296,10 +1273,10 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
@@ -1308,10 +1285,10 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1322,10 +1299,10 @@
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1356,36 +1333,36 @@
       <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="21">
@@ -1592,13 +1569,13 @@
       </c>
       <c r="C24" s="36"/>
       <c r="D24" s="37"/>
-      <c r="E24" s="69" t="s">
+      <c r="E24" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="27">
@@ -1712,13 +1689,13 @@
       <c r="D30" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="61" t="s">
+      <c r="E30" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="70"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="27">
@@ -1746,13 +1723,13 @@
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="30"/>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
     </row>
     <row r="33" spans="1:9" ht="26.5" customHeight="1">
       <c r="A33" s="27">
@@ -1766,13 +1743,13 @@
       <c r="D33" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="65" t="s">
+      <c r="E33" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
     </row>
     <row r="34" spans="1:9" ht="14" customHeight="1">
       <c r="A34" s="27">
@@ -1784,13 +1761,13 @@
       </c>
       <c r="C34" s="36"/>
       <c r="D34" s="37"/>
-      <c r="E34" s="65" t="s">
+      <c r="E34" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
     </row>
     <row r="35" spans="1:9" ht="14" customHeight="1">
       <c r="A35" s="27">
@@ -1804,13 +1781,13 @@
       <c r="D35" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="57" t="s">
+      <c r="E35" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="59"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="66"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="27">
@@ -1864,13 +1841,13 @@
       <c r="D38" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="54" t="s">
+      <c r="E38" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="63"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="27">
@@ -1884,33 +1861,24 @@
       <c r="D39" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="54" t="s">
+      <c r="E39" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="56"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="63"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="27">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>81</v>
-      </c>
+      <c r="A40" s="27"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="36"/>
-      <c r="D40" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="56"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="63"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="39"/>
@@ -1925,6 +1893,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E39:I39"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -1936,13 +1911,6 @@
     <mergeCell ref="E24:I24"/>
     <mergeCell ref="E32:I32"/>
     <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E39:I39"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">

</xml_diff>